<commit_message>
Added Continuous Lab support.
</commit_message>
<xml_diff>
--- a/AWSCloudLabCore/deployment/namelist/ITP4104 Lab A.xlsx
+++ b/AWSCloudLabCore/deployment/namelist/ITP4104 Lab A.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>key</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>awsAccount</t>
-  </si>
-  <si>
-    <t>win2012ssh</t>
   </si>
   <si>
     <t>email</t>
@@ -409,60 +403,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>